<commit_message>
added default template file
</commit_message>
<xml_diff>
--- a/react_template.xlsx
+++ b/react_template.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maury\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Components</t>
   </si>
@@ -75,6 +80,9 @@
     <t>library</t>
   </si>
   <si>
+    <t>materialUI</t>
+  </si>
+  <si>
     <t>layout</t>
   </si>
   <si>
@@ -83,120 +91,12 @@
   <si>
     <t>value8</t>
   </si>
-  <si>
-    <t>Chart</t>
-  </si>
-  <si>
-    <t>DropDown</t>
-  </si>
-  <si>
-    <t>TextInput</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customer First Name: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customer middle  Name: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customer Last Name: </t>
-  </si>
-  <si>
-    <t>custName</t>
-  </si>
-  <si>
-    <t>middle name</t>
-  </si>
-  <si>
-    <t>custLastName</t>
-  </si>
-  <si>
-    <t>RadioButton</t>
-  </si>
-  <si>
-    <t>CheckBox</t>
-  </si>
-  <si>
-    <t>Gender:</t>
-  </si>
-  <si>
-    <t>Marital Status</t>
-  </si>
-  <si>
-    <t>Languages</t>
-  </si>
-  <si>
-    <t>Do you own any policy with us?</t>
-  </si>
-  <si>
-    <t>Renewed Policies</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>maritalStatus</t>
-  </si>
-  <si>
-    <t>languages</t>
-  </si>
-  <si>
-    <t>ownPolicy</t>
-  </si>
-  <si>
-    <t>Bar</t>
-  </si>
-  <si>
-    <t>Pie</t>
-  </si>
-  <si>
-    <t>{"labels":["January", "February", "March", "April", "May", "June"],"datasets":[{"label":"# of Policies Renewed","data":[12,19,3,5,2,3],"backgroundColor":["rgba(255, 99, 132, 0.2)","rgba(54, 162, 235, 0.2)","rgba(255, 206, 86, 0.2)","rgba(75, 192, 192, 0.2)","rgba(153, 102, 255, 0.2)","rgba(255, 159, 64, 0.2)"],"borderColor":["rgba(255, 99, 132, 1)","rgba(54, 162, 235, 1)","rgba(255, 206, 86, 1)","rgba(75, 192, 192, 1)","rgba(153, 102, 255, 1)","rgba(255, 159, 64, 1)"],"borderWidth":1}]}</t>
-  </si>
-  <si>
-    <t>options</t>
-  </si>
-  <si>
-    <t>{"maintainAspectRatio": false, "scales":{"yAxes":[{"ticks":{"beginAtZero":true}}]}}</t>
-  </si>
-  <si>
-    <t>Male,Female,Other</t>
-  </si>
-  <si>
-    <t>Married,Unmarried,Other</t>
-  </si>
-  <si>
-    <t>English,Hindi,Spanish,Chinese,Other</t>
-  </si>
-  <si>
-    <t>Yes,No</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>DemoApp</t>
-  </si>
-  <si>
-    <t>row</t>
-  </si>
-  <si>
-    <t>primeReact</t>
-  </si>
-  <si>
-    <t>child</t>
-  </si>
-  <si>
-    <t>child-row</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,10 +137,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -301,7 +200,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -336,7 +235,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -513,43 +412,43 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.1796875" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" customWidth="1"/>
+    <col min="5" max="5" width="18.08984375" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" customWidth="1"/>
-    <col min="12" max="12" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" customWidth="1"/>
-    <col min="16" max="16" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.140625" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" customWidth="1"/>
+    <col min="8" max="8" width="13.08984375" customWidth="1"/>
+    <col min="9" max="9" width="16.1796875" customWidth="1"/>
+    <col min="10" max="10" width="12.7265625" customWidth="1"/>
+    <col min="11" max="11" width="17.36328125" customWidth="1"/>
+    <col min="12" max="12" width="10.6328125" customWidth="1"/>
+    <col min="13" max="13" width="12.81640625" customWidth="1"/>
+    <col min="14" max="14" width="11.81640625" customWidth="1"/>
+    <col min="15" max="15" width="10.54296875" customWidth="1"/>
+    <col min="16" max="16" width="12.453125" customWidth="1"/>
+    <col min="17" max="17" width="10.1796875" customWidth="1"/>
+    <col min="18" max="18" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,155 +498,110 @@
         <v>9</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C57" si="0">IF($A3="TextContainer","label",IF($A3="TextInput","label",IF($A3="CheckBox","label",IF($A3="DropDown","label",IF($A3="RadioButton","label",IF($A3="Chart","label",IF($A3="Table","stickyHeader","")))))))</f>
-        <v>label</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
+        <f>IF($A3="TextContainer","label",IF($A3="TextInput","label",IF($A3="CheckBox","label",IF($A3="DropDown","label",IF($A3="RadioButton","label",IF($A3="Chart","label",IF($A3="Table","stickyHeader","")))))))</f>
+        <v/>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E57" si="1">IF($A3="TextContainer","",IF($A3="TextInput","id",IF($A3="CheckBox","id",IF($A3="DropDown","id",IF($A3="RadioButton","id",IF($A3="Chart","id",IF($A3="Table","id","")))))))</f>
-        <v>id</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
+        <f>IF($A3="TextContainer","",IF($A3="TextInput","id",IF($A3="CheckBox","id",IF($A3="DropDown","id",IF($A3="RadioButton","id",IF($A3="Chart","id",IF($A3="Table","id","")))))))</f>
+        <v/>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G57" si="2">IF($A3="TextContainer","mandatory",IF($A3="TextInput","mandatory",IF($A3="CheckBox","mandatory",IF($A3="DropDown","mandatory",IF($A3="RadioButton","mandatory",IF($A3="Chart","type",IF($A3="Table","","")))))))</f>
-        <v>mandatory</v>
-      </c>
-      <c r="H3" t="b">
-        <v>1</v>
+        <f>IF($A3="TextContainer","mandatory",IF($A3="TextInput","mandatory",IF($A3="CheckBox","mandatory",IF($A3="DropDown","mandatory",IF($A3="RadioButton","mandatory",IF($A3="Chart","type",IF($A3="Table","","")))))))</f>
+        <v/>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I57" si="3">IF($A3="TextContainer","",IF($A3="TextInput","default",IF($A3="CheckBox","default",IF($A3="DropDown","default",IF($A3="RadioButton","default",IF($A3="Chart","",IF($A3="","","")))))))</f>
-        <v>default</v>
+        <f>IF($A3="TextContainer","",IF($A3="TextInput","default",IF($A3="CheckBox","default",IF($A3="DropDown","default",IF($A3="RadioButton","default",IF($A3="Chart","",IF($A3="","","")))))))</f>
+        <v/>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K57" si="4">IF($A3="TextContainer","",IF($A3="TextInput","",IF($A3="CheckBox","options",IF($A3="DropDown","options",IF($A3="RadioButton","options",IF($A3="Chart","",IF($A3="Table","","")))))))</f>
+        <f>IF($A3="TextContainer","",IF($A3="TextInput","",IF($A3="CheckBox","options",IF($A3="DropDown","options",IF($A3="RadioButton","options",IF($A3="Chart","",IF($A3="Table","","")))))))</f>
         <v/>
       </c>
       <c r="M3" t="str">
-        <f t="shared" ref="M3:M57" si="5">IF($A3="TextContainer","",IF($A3="TextInput","",IF($A3="CheckBox","api",IF($A3="DropDown","api",IF($A3="RadioButton","api",IF($A3="Chart","api",IF($A3="Table","api","")))))))</f>
+        <f>IF($A3="TextContainer","",IF($A3="TextInput","",IF($A3="CheckBox","api",IF($A3="DropDown","api",IF($A3="RadioButton","api",IF($A3="Chart","api",IF($A3="Table","api","")))))))</f>
         <v/>
       </c>
       <c r="O3" t="str">
-        <f t="shared" ref="O3:O57" si="6">IF($A3="TextContainer","",IF($A3="TextInput","",IF($A3="CheckBox","",IF($A3="DropDown","",IF($A3="RadioButton","",IF($A3="Chart","data",IF($A3="Table","data","")))))))</f>
+        <f>IF($A3="TextContainer","",IF($A3="TextInput","",IF($A3="CheckBox","",IF($A3="DropDown","",IF($A3="RadioButton","",IF($A3="Chart","data",IF($A3="Table","data","")))))))</f>
         <v/>
       </c>
       <c r="Q3" t="str">
-        <f t="shared" ref="Q3:Q56" si="7">IF($A3="TextContainer","className",IF($A3="TextInput","className",IF($A3="CheckBox","className",IF($A3="DropDown","className",IF($A3="RadioButton","className",IF($A3="Chart","className",IF($A3="Table","className","")))))))</f>
-        <v>className</v>
-      </c>
-      <c r="R3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
+        <f>IF($A3="TextContainer","className",IF($A3="TextInput","className",IF($A3="CheckBox","className",IF($A3="DropDown","className",IF($A3="RadioButton","className",IF($A3="Chart","className",IF($A3="Table","className","")))))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C4" t="str">
-        <f t="shared" si="0"/>
-        <v>label</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
+        <f t="shared" ref="C4:C60" si="0">IF($A4="TextContainer","label",IF($A4="TextInput","label",IF($A4="CheckBox","label",IF($A4="DropDown","label",IF($A4="RadioButton","label",IF($A4="Chart","label",IF($A4="Table","stickyHeader","")))))))</f>
+        <v/>
       </c>
       <c r="E4" t="str">
-        <f t="shared" si="1"/>
-        <v>id</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
+        <f t="shared" ref="E4:E60" si="1">IF($A4="TextContainer","",IF($A4="TextInput","id",IF($A4="CheckBox","id",IF($A4="DropDown","id",IF($A4="RadioButton","id",IF($A4="Chart","id",IF($A4="Table","id","")))))))</f>
+        <v/>
       </c>
       <c r="G4" t="str">
-        <f t="shared" si="2"/>
-        <v>mandatory</v>
+        <f t="shared" ref="G4:G60" si="2">IF($A4="TextContainer","mandatory",IF($A4="TextInput","mandatory",IF($A4="CheckBox","mandatory",IF($A4="DropDown","mandatory",IF($A4="RadioButton","mandatory",IF($A4="Chart","type",IF($A4="Table","","")))))))</f>
+        <v/>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="3"/>
-        <v>default</v>
+        <f t="shared" ref="I4:I60" si="3">IF($A4="TextContainer","",IF($A4="TextInput","default",IF($A4="CheckBox","default",IF($A4="DropDown","default",IF($A4="RadioButton","default",IF($A4="Chart","",IF($A4="","","")))))))</f>
+        <v/>
       </c>
       <c r="K4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="K4:K60" si="4">IF($A4="TextContainer","",IF($A4="TextInput","",IF($A4="CheckBox","options",IF($A4="DropDown","options",IF($A4="RadioButton","options",IF($A4="Chart","",IF($A4="Table","","")))))))</f>
         <v/>
       </c>
       <c r="M4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="M4:M60" si="5">IF($A4="TextContainer","",IF($A4="TextInput","",IF($A4="CheckBox","api",IF($A4="DropDown","api",IF($A4="RadioButton","api",IF($A4="Chart","api",IF($A4="Table","api","")))))))</f>
         <v/>
       </c>
       <c r="O4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="O4:O60" si="6">IF($A4="TextContainer","",IF($A4="TextInput","",IF($A4="CheckBox","",IF($A4="DropDown","",IF($A4="RadioButton","",IF($A4="Chart","data",IF($A4="Table","data","")))))))</f>
         <v/>
       </c>
       <c r="Q4" t="str">
-        <f t="shared" si="7"/>
-        <v>className</v>
-      </c>
-      <c r="R4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
+        <f t="shared" ref="Q4:Q59" si="7">IF($A4="TextContainer","className",IF($A4="TextInput","className",IF($A4="CheckBox","className",IF($A4="DropDown","className",IF($A4="RadioButton","className",IF($A4="Chart","className",IF($A4="Table","className","")))))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>label</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
+        <v/>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="1"/>
-        <v>id</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
+        <v/>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="2"/>
-        <v>mandatory</v>
-      </c>
-      <c r="H5" t="b">
-        <v>1</v>
+        <v/>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="3"/>
-        <v>default</v>
+        <v/>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="4"/>
@@ -763,54 +617,33 @@
       </c>
       <c r="Q5" t="str">
         <f t="shared" si="7"/>
-        <v>className</v>
-      </c>
-      <c r="R5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v>label</v>
-      </c>
-      <c r="D6" t="s">
-        <v>32</v>
+        <v/>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="1"/>
-        <v>id</v>
-      </c>
-      <c r="F6" t="s">
-        <v>37</v>
+        <v/>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="2"/>
-        <v>mandatory</v>
-      </c>
-      <c r="H6" t="b">
-        <v>0</v>
+        <v/>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="3"/>
-        <v>default</v>
-      </c>
-      <c r="J6" t="s">
-        <v>50</v>
+        <v/>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="4"/>
-        <v>options</v>
-      </c>
-      <c r="L6" t="s">
-        <v>46</v>
+        <v/>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="5"/>
-        <v>api</v>
+        <v/>
       </c>
       <c r="O6" t="str">
         <f t="shared" si="6"/>
@@ -818,51 +651,33 @@
       </c>
       <c r="Q6" t="str">
         <f t="shared" si="7"/>
-        <v>className</v>
-      </c>
-      <c r="R6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>label</v>
-      </c>
-      <c r="D7" t="s">
-        <v>33</v>
+        <v/>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="1"/>
-        <v>id</v>
-      </c>
-      <c r="F7" t="s">
-        <v>38</v>
+        <v/>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="2"/>
-        <v>mandatory</v>
-      </c>
-      <c r="H7" t="b">
-        <v>1</v>
+        <v/>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="3"/>
-        <v>default</v>
+        <v/>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="4"/>
-        <v>options</v>
-      </c>
-      <c r="L7" t="s">
-        <v>47</v>
+        <v/>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="5"/>
-        <v>api</v>
+        <v/>
       </c>
       <c r="O7" t="str">
         <f t="shared" si="6"/>
@@ -870,54 +685,33 @@
       </c>
       <c r="Q7" t="str">
         <f t="shared" si="7"/>
-        <v>className</v>
-      </c>
-      <c r="R7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C8" t="str">
-        <f>IF($A8="TextContainer","label",IF($A8="TextInput","label",IF($A8="CheckBox","label",IF($A8="DropDown","label",IF($A8="RadioButton","label",IF($A8="Chart","label",IF($A8="Table","stickyHeader","")))))))</f>
-        <v>label</v>
-      </c>
-      <c r="D8" t="s">
-        <v>34</v>
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="1"/>
-        <v>id</v>
-      </c>
-      <c r="F8" t="s">
-        <v>39</v>
+        <v/>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="2"/>
-        <v>mandatory</v>
-      </c>
-      <c r="H8" t="b">
-        <v>1</v>
+        <v/>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="3"/>
-        <v>default</v>
-      </c>
-      <c r="J8" t="s">
-        <v>51</v>
+        <v/>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="4"/>
-        <v>options</v>
-      </c>
-      <c r="L8" t="s">
-        <v>48</v>
+        <v/>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="5"/>
-        <v>api</v>
+        <v/>
       </c>
       <c r="O8" t="str">
         <f t="shared" si="6"/>
@@ -925,51 +719,33 @@
       </c>
       <c r="Q8" t="str">
         <f t="shared" si="7"/>
-        <v>className</v>
-      </c>
-      <c r="R8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C9" t="str">
-        <f t="shared" si="0"/>
-        <v>label</v>
-      </c>
-      <c r="D9" t="s">
-        <v>35</v>
+        <f>IF($A9="TextContainer","label",IF($A9="TextInput","label",IF($A9="CheckBox","label",IF($A9="DropDown","label",IF($A9="RadioButton","label",IF($A9="Chart","label",IF($A9="Table","stickyHeader","")))))))</f>
+        <v/>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
-        <v>id</v>
-      </c>
-      <c r="F9" t="s">
-        <v>40</v>
+        <v/>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="2"/>
-        <v>mandatory</v>
-      </c>
-      <c r="H9" t="b">
-        <v>0</v>
+        <v/>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="3"/>
-        <v>default</v>
+        <v/>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="4"/>
-        <v>options</v>
-      </c>
-      <c r="L9" t="s">
-        <v>49</v>
+        <v/>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="5"/>
-        <v>api</v>
+        <v/>
       </c>
       <c r="O9" t="str">
         <f t="shared" si="6"/>
@@ -977,36 +753,21 @@
       </c>
       <c r="Q9" t="str">
         <f t="shared" si="7"/>
-        <v>className</v>
-      </c>
-      <c r="R9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>label</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
+        <v/>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
-        <v>id</v>
-      </c>
-      <c r="F10" t="s">
-        <v>41</v>
+        <v/>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="2"/>
-        <v>type</v>
-      </c>
-      <c r="H10" t="s">
-        <v>41</v>
+        <v/>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="3"/>
@@ -1018,46 +779,29 @@
       </c>
       <c r="M10" t="str">
         <f t="shared" si="5"/>
-        <v>api</v>
+        <v/>
       </c>
       <c r="O10" t="str">
         <f t="shared" si="6"/>
-        <v>data</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="R10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
+        <v/>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>label</v>
-      </c>
-      <c r="D11" t="s">
-        <v>36</v>
+        <v/>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
-        <v>id</v>
-      </c>
-      <c r="F11" t="s">
-        <v>42</v>
+        <v/>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="2"/>
-        <v>type</v>
-      </c>
-      <c r="H11" t="s">
-        <v>42</v>
+        <v/>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="3"/>
@@ -1069,23 +813,18 @@
       </c>
       <c r="M11" t="str">
         <f t="shared" si="5"/>
-        <v>api</v>
+        <v/>
       </c>
       <c r="O11" t="str">
         <f t="shared" si="6"/>
-        <v>data</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="R11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
+        <v/>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1119,7 +858,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1153,7 +892,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1187,7 +926,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1221,7 +960,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1255,7 +994,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="3:17">
+    <row r="17" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1289,7 +1028,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="3:17">
+    <row r="18" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1323,7 +1062,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="3:17">
+    <row r="19" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1357,7 +1096,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="3:17">
+    <row r="20" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1391,7 +1130,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="3:17">
+    <row r="21" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C21" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1425,7 +1164,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="3:17">
+    <row r="22" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C22" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1459,7 +1198,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="3:17">
+    <row r="23" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C23" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1493,7 +1232,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="3:17">
+    <row r="24" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C24" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1527,7 +1266,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="3:17">
+    <row r="25" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C25" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1561,7 +1300,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="3:17">
+    <row r="26" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C26" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1595,7 +1334,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="3:17">
+    <row r="27" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C27" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1629,7 +1368,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="3:17">
+    <row r="28" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C28" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1663,7 +1402,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="3:17">
+    <row r="29" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C29" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1697,7 +1436,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="3:17">
+    <row r="30" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C30" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1731,7 +1470,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="3:17">
+    <row r="31" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C31" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1765,7 +1504,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="3:17">
+    <row r="32" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C32" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1799,7 +1538,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="3:17">
+    <row r="33" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C33" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1829,11 +1568,11 @@
         <v/>
       </c>
       <c r="Q33" t="str">
-        <f>IF($A33="TextContainer","className",IF($A33="TextInput","className",IF($A33="CheckBox","className",IF($A33="DropDown","className",IF($A33="RadioButton","className",IF($A33="Chart","className",IF($A33="Table","className","")))))))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="3:17">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C34" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1867,7 +1606,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="3:17">
+    <row r="35" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C35" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1901,7 +1640,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="3:17">
+    <row r="36" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C36" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1931,11 +1670,11 @@
         <v/>
       </c>
       <c r="Q36" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="3:17">
+        <f>IF($A36="TextContainer","className",IF($A36="TextInput","className",IF($A36="CheckBox","className",IF($A36="DropDown","className",IF($A36="RadioButton","className",IF($A36="Chart","className",IF($A36="Table","className","")))))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C37" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1969,7 +1708,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="3:17">
+    <row r="38" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C38" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2003,7 +1742,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="3:17">
+    <row r="39" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C39" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2037,7 +1776,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="3:17">
+    <row r="40" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C40" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2071,7 +1810,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="3:17">
+    <row r="41" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C41" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2105,7 +1844,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="3:17">
+    <row r="42" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C42" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2139,7 +1878,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="3:17">
+    <row r="43" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C43" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2173,7 +1912,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="3:17">
+    <row r="44" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2207,7 +1946,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="3:17">
+    <row r="45" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C45" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2241,7 +1980,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="3:17">
+    <row r="46" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C46" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2275,7 +2014,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="3:17">
+    <row r="47" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C47" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2309,7 +2048,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="3:17">
+    <row r="48" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C48" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2339,11 +2078,11 @@
         <v/>
       </c>
       <c r="Q48" t="str">
-        <f>IF($A48="TextContainer","className",IF($A48="TextInput","className",IF($A48="CheckBox","className",IF($A48="DropDown","className",IF($A48="RadioButton","className",IF($A48="Chart","className",IF($A48="Table","className","")))))))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="3:17">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C49" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2377,7 +2116,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="3:17">
+    <row r="50" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C50" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2411,7 +2150,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="3:17">
+    <row r="51" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C51" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2441,11 +2180,11 @@
         <v/>
       </c>
       <c r="Q51" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="3:17">
+        <f>IF($A51="TextContainer","className",IF($A51="TextInput","className",IF($A51="CheckBox","className",IF($A51="DropDown","className",IF($A51="RadioButton","className",IF($A51="Chart","className",IF($A51="Table","className","")))))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C52" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2479,7 +2218,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="3:17">
+    <row r="53" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C53" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2513,7 +2252,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="3:17">
+    <row r="54" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C54" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2547,7 +2286,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="3:17">
+    <row r="55" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C55" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2581,7 +2320,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="3:17">
+    <row r="56" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C56" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2603,7 +2342,7 @@
         <v/>
       </c>
       <c r="M56" t="str">
-        <f>IF($A56="TextContainer","",IF($A56="TextInput","",IF($A56="CheckBox","api",IF($A56="DropDown","api",IF($A56="RadioButton","api",IF($A56="Chart","api",IF($A56="Table","api","")))))))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O56" t="str">
@@ -2615,7 +2354,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="3:17">
+    <row r="57" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C57" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2645,22 +2384,124 @@
         <v/>
       </c>
       <c r="Q57" t="str">
-        <f>IF($A57="TextContainer","className",IF($A57="TextInput","className",IF($A57="CheckBox","className",IF($A57="DropDown","className",IF($A57="RadioButton","className",IF($A57="Chart","className",IF($A57="Table","className","")))))))</f>
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I58" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K58" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M58" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O58" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q58" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I59" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K59" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M59" t="str">
+        <f>IF($A59="TextContainer","",IF($A59="TextInput","",IF($A59="CheckBox","api",IF($A59="DropDown","api",IF($A59="RadioButton","api",IF($A59="Chart","api",IF($A59="Table","api","")))))))</f>
+        <v/>
+      </c>
+      <c r="O59" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q59" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I60" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K60" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M60" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O60" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q60" t="str">
+        <f>IF($A60="TextContainer","className",IF($A60="TextInput","className",IF($A60="CheckBox","className",IF($A60="DropDown","className",IF($A60="RadioButton","className",IF($A60="Chart","className",IF($A60="Table","className","")))))))</f>
         <v/>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A57">
-      <formula1>"CheckBox,DropDown,TestInput,RadioButton,Chart,Table,TextContainer"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
       <formula1>"materialUI,primeReact"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
       <formula1>"row,column"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A56">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A60">
+      <formula1>"CheckBox,DropDown,TestInput,RadioButton,Chart,Table,TextContainer"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A59">
       <formula1>"CheckBox,DropDown,TextInput,RadioButton,Chart,Table,TextContainer"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>